<commit_message>
Experimental support for literals
</commit_message>
<xml_diff>
--- a/doc/Transitionstabelle.xlsx
+++ b/doc/Transitionstabelle.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CONSTANT</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>[^A-Za-z0-9_:-]</t>
+  </si>
+  <si>
+    <t>LITERAL</t>
+  </si>
+  <si>
+    <t>'</t>
   </si>
 </sst>
 </file>
@@ -447,18 +453,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I8"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="10" width="17.1640625" customWidth="1"/>
+    <col min="2" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="C2" t="s">
         <v>2</v>
       </c>
@@ -478,10 +484,13 @@
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:10">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -497,12 +506,12 @@
         <f>B5</f>
         <v>VARIABLE</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <f>B6</f>
         <v>SPECIAL_CHAR</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -515,19 +524,19 @@
         <v>CONSTANT</v>
       </c>
       <c r="F4" t="str">
-        <f>B7</f>
+        <f>B8</f>
         <v>COLON</v>
       </c>
       <c r="H4" t="str">
         <f>B4</f>
         <v>CONSTANT</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f>B6</f>
         <v>SPECIAL_CHAR</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -547,12 +556,12 @@
         <f>B5</f>
         <v>VARIABLE</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f>B6</f>
         <v>SPECIAL_CHAR</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -569,7 +578,7 @@
         <v>CONSTANT</v>
       </c>
       <c r="F6" t="str">
-        <f>B7</f>
+        <f>B8</f>
         <v>COLON</v>
       </c>
       <c r="H6" t="str">
@@ -577,36 +586,81 @@
         <v>CONSTANT</v>
       </c>
       <c r="I6" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="J6" t="str">
         <f>B6</f>
         <v>SPECIAL_CHAR</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="D7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="E7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="F7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="G7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="H7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="I7" t="str">
+        <f>B3</f>
+        <v>INIT</v>
+      </c>
+      <c r="J7" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="str">
-        <f>B8</f>
+      <c r="G8" t="str">
+        <f>B9</f>
         <v>DASH</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="str">
-        <f>B4</f>
-        <v>CONSTANT</v>
-      </c>
-      <c r="D8" t="str">
-        <f>B5</f>
-        <v>VARIABLE</v>
-      </c>
-      <c r="E8" t="str">
-        <f>B4</f>
-        <v>CONSTANT</v>
-      </c>
-      <c r="I8" t="str">
+      <c r="C9" t="str">
+        <f>B4</f>
+        <v>CONSTANT</v>
+      </c>
+      <c r="D9" t="str">
+        <f>B5</f>
+        <v>VARIABLE</v>
+      </c>
+      <c r="E9" t="str">
+        <f>B4</f>
+        <v>CONSTANT</v>
+      </c>
+      <c r="I9" t="str">
+        <f>B7</f>
+        <v>LITERAL</v>
+      </c>
+      <c r="J9" t="str">
         <f>B6</f>
         <v>SPECIAL_CHAR</v>
       </c>

</xml_diff>